<commit_message>
corrected spelling of perturbbation
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_H.BROWN_09.17.19.xlsx
+++ b/bioSample/bioSample_H.BROWN_09.17.19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B235136-FB89-604C-A5F7-6A5214AABD01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B679C33-F730-2D45-BCAA-E310DC83660C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,7 +111,7 @@
     <t>NAT</t>
   </si>
   <si>
-    <t>Environmental_Pertubation</t>
+    <t>Environmental_Perturbation</t>
   </si>
 </sst>
 </file>

</xml_diff>